<commit_message>
Pushing changes to sync with LM
</commit_message>
<xml_diff>
--- a/Input/MATSimWIMInput.xlsx
+++ b/Input/MATSimWIMInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsja\Desktop\SwissTraffic\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5FADE3-DEBA-42C6-A56A-EC83DBF744B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF11D01-C1A7-47D8-9D9B-BAE8308494FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="14616" tabRatio="813" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>RunDyn</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>V,Mp,Mn</t>
+  </si>
+  <si>
+    <t>Ceneri</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,10 +543,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3">
-        <v>2011</v>
+        <v>2018</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -584,10 +587,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -620,6 +623,94 @@
         <v>0</v>
       </c>
       <c r="N3" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2017</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2018</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Try to get baseline
</commit_message>
<xml_diff>
--- a/Input/MATSimWIMInput.xlsx
+++ b/Input/MATSimWIMInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsja\Desktop\SwissTraffic\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF11D01-C1A7-47D8-9D9B-BAE8308494FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02A2A43-BB19-425B-8EDD-9DB743CE0A3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="14616" tabRatio="813" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="948" yWindow="24" windowWidth="22092" windowHeight="14376" tabRatio="813" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseData" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>RunDyn</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Folder</t>
-  </si>
-  <si>
-    <t>Denges</t>
   </si>
   <si>
     <t>SName</t>
@@ -473,10 +470,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,10 +496,10 @@
         <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>7</v>
@@ -532,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -543,13 +540,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -561,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2">
         <v>1</v>
@@ -587,13 +584,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3">
         <v>2017</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -605,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
@@ -623,94 +620,6 @@
         <v>0</v>
       </c>
       <c r="N3" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2017</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2018</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
         <v>10</v>
       </c>
     </row>

</xml_diff>